<commit_message>
Updated value to XLSX and based on the files used last year, as some files have been changed.
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -2,9 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mikkel Simonsen\TIMES-DK\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="285" yWindow="45" windowWidth="9705" windowHeight="7305" tabRatio="853" activeTab="2"/>
+    <workbookView xWindow="285" yWindow="30" windowWidth="9690" windowHeight="7290" tabRatio="853" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -28,7 +33,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
     <comment ref="B4" authorId="0" shapeId="0">
@@ -51,65 +56,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
-  </authors>
-  <commentList>
-    <comment ref="D3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>If more periods definition are created, user can change them</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>More time periods definition from here</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Author</author>
+    <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
     <comment ref="G6" authorId="0" shapeId="0">
@@ -410,7 +357,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -475,20 +422,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -540,6 +481,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA72EC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -612,7 +565,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -625,7 +578,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -654,6 +606,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1304,10 +1259,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1316,79 +1271,82 @@
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="4">
-        <v>2012</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="4">
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="4">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="4">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="4">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="4">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="4">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="4">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="4">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="4">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="30">
         <v>5</v>
       </c>
     </row>
@@ -1397,7 +1355,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1405,7 +1362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
@@ -1413,31 +1370,31 @@
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="5" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
@@ -1496,10 +1453,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6" t="s">
@@ -1522,22 +1479,22 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="13" spans="2:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="18" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
@@ -1642,11 +1599,11 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.140625" customWidth="1"/>
+    <col min="7" max="8" width="11.28515625" customWidth="1"/>
     <col min="9" max="11" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1660,24 +1617,24 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="4" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -1703,22 +1660,22 @@
       <c r="G6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="24" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="26"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1740,7 +1697,7 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
@@ -1806,26 +1763,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="21"/>
-    <col min="2" max="2" width="12.140625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="14" style="21" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" style="21" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="21" customWidth="1"/>
-    <col min="10" max="10" width="11" style="21" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" width="9.140625" style="20"/>
+    <col min="2" max="2" width="12.140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="14" style="20" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="11" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1883,37 +1840,37 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="20" t="s">
         <v>51</v>
       </c>
       <c r="E7"/>
-      <c r="H7" s="22">
+      <c r="H7" s="21">
         <v>0.05</v>
       </c>
-      <c r="I7" s="22"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>61</v>
       </c>
       <c r="E8"/>
-      <c r="H8" s="22">
+      <c r="H8" s="21">
         <v>1</v>
       </c>
-      <c r="I8" s="22"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>72</v>
       </c>
       <c r="E9"/>
-      <c r="H9" s="22">
+      <c r="H9" s="21">
         <v>2012</v>
       </c>
-      <c r="I9" s="22"/>
+      <c r="I9" s="21"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10"/>
@@ -1921,16 +1878,16 @@
       <c r="D10" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="21" t="str">
+      <c r="F10" s="20" t="str">
         <f>Defaults!$B$4</f>
         <v>MEUR2012</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="27">
         <f>1/0.971011369084674</f>
         <v>1.0298540592193604</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="R10" s="21" t="str">
+      <c r="I10" s="21"/>
+      <c r="R10" s="20" t="str">
         <f>Defaults!B5</f>
         <v>MEUR2010</v>
       </c>
@@ -1941,16 +1898,16 @@
       <c r="D11" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="21" t="str">
+      <c r="F11" s="20" t="str">
         <f>Defaults!$B$4</f>
         <v>MEUR2012</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="27">
         <f>1/0.976646137384215</f>
         <v>1.0239123073566179</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="R11" s="21" t="str">
+      <c r="I11" s="21"/>
+      <c r="R11" s="20" t="str">
         <f>Defaults!B6</f>
         <v>MEUR2011</v>
       </c>
@@ -1961,16 +1918,16 @@
       <c r="D12" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="21" t="str">
+      <c r="F12" s="20" t="str">
         <f>Defaults!$B$4</f>
         <v>MEUR2012</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="27">
         <f>1/1.01705478454671</f>
         <v>0.98323120366194328</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="R12" s="21" t="str">
+      <c r="I12" s="21"/>
+      <c r="R12" s="20" t="str">
         <f>Defaults!B7</f>
         <v>MEUR2013</v>
       </c>
@@ -1981,16 +1938,16 @@
       <c r="D13" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="21" t="str">
+      <c r="F13" s="20" t="str">
         <f>Defaults!$B$4</f>
         <v>MEUR2012</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="27">
         <f>1/1.02306606930474</f>
         <v>0.97745397878319307</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="R13" s="21" t="str">
+      <c r="I13" s="21"/>
+      <c r="R13" s="20" t="str">
         <f>Defaults!B8</f>
         <v>MEUR2014</v>
       </c>
@@ -2001,16 +1958,16 @@
       <c r="D14" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="21" t="str">
+      <c r="F14" s="20" t="str">
         <f>Defaults!$B$4</f>
         <v>MEUR2012</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="27">
         <f>1/1.03379387534522</f>
         <v>0.96731081877039071</v>
       </c>
-      <c r="I14" s="22"/>
-      <c r="R14" s="21" t="str">
+      <c r="I14" s="21"/>
+      <c r="R14" s="20" t="str">
         <f>Defaults!B9</f>
         <v>MEUR2015</v>
       </c>
@@ -2021,14 +1978,14 @@
       <c r="D15" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="20">
         <v>2012</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="21">
         <v>0.92</v>
       </c>
-      <c r="I15" s="22"/>
-      <c r="P15" s="21" t="s">
+      <c r="I15" s="21"/>
+      <c r="P15" s="20" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2038,14 +1995,14 @@
       <c r="D16" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="20">
         <v>2012</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="21">
         <v>0.8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="P16" s="21" t="s">
+      <c r="I16" s="21"/>
+      <c r="P16" s="20" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2053,36 +2010,36 @@
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
+      <c r="B20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
+      <c r="B21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2114,22 +2071,22 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="26" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2175,6 +2132,5 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
 </worksheet>
 </file>
</xml_diff>